<commit_message>
Add NoPattern Case Analysis
</commit_message>
<xml_diff>
--- a/NoPatternCaseAnalysis.xlsx
+++ b/NoPatternCaseAnalysis.xlsx
@@ -1,6 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr date1904="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Table 1</t>
   </si>
@@ -37,7 +38,79 @@
     <t>jdt</t>
   </si>
   <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>Super class was deleted; one method in super class injected to two subclasses; this method cant be detected by changes distiller</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Subtle corn, throws same exception</t>
+  </si>
+  <si>
+    <t>Corn, should be detected.</t>
+  </si>
+  <si>
+    <t>Dependencies not extracted by Understand at the method level</t>
+  </si>
+  <si>
+    <t>NoPatternFound</t>
+  </si>
+  <si>
+    <t>NoPatternFound manually</t>
+  </si>
+  <si>
+    <t>Corn or Lambda(call same thing, called is not changed)</t>
+  </si>
+  <si>
+    <t>NoPatternFound manually; every two files have similar changes</t>
+  </si>
+  <si>
+    <t>methods in new files can not be extracted</t>
+  </si>
+  <si>
+    <t>this.expression.isPolyExpression() cant be extracted by Understand</t>
+  </si>
+  <si>
+    <t>Tiny patches together</t>
+  </si>
+  <si>
+    <t>Upsilon</t>
+  </si>
+  <si>
+    <t>Changes not detected</t>
+  </si>
+  <si>
+    <t>Corn, should be detected. if() system.out</t>
+  </si>
+  <si>
     <t>p2</t>
+  </si>
+  <si>
+    <t>Corn, should be detected. Fields added in multiple places</t>
+  </si>
+  <si>
+    <t>NoPatternFound or Corn</t>
+  </si>
+  <si>
+    <t>remove type, okay</t>
+  </si>
+  <si>
+    <t>changes  declare; okay</t>
+  </si>
+  <si>
+    <t>corn may not be detected; method name slightly different</t>
+  </si>
+  <si>
+    <t>Dependencies not extracted by Understand at the method level; should be improved by matching changed method names</t>
   </si>
   <si>
     <t>swt</t>
@@ -219,7 +292,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -238,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -251,6 +324,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1383,7 +1459,7 @@
     <col min="3" max="3" width="20.8516" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.375" style="1" customWidth="1"/>
     <col min="7" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1424,10 +1500,18 @@
       <c r="B3" s="5">
         <v>401847</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="C3" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" ht="20.35" customHeight="1">
       <c r="A4" t="s" s="7">
@@ -1484,10 +1568,18 @@
       <c r="B8" s="10">
         <v>507571</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="C8" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s" s="11">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="A9" t="s" s="7">
@@ -1544,10 +1636,18 @@
       <c r="B13" s="10">
         <v>474239</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="C13" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s" s="11">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" t="s" s="7">
@@ -1604,10 +1704,18 @@
       <c r="B18" s="10">
         <v>430136</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="C18" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s" s="11">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" ht="20.35" customHeight="1">
       <c r="A19" t="s" s="7">
@@ -1664,10 +1772,18 @@
       <c r="B23" s="10">
         <v>426537</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="C23" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s" s="11">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s" s="11">
+        <v>17</v>
+      </c>
     </row>
     <row r="24" ht="20.35" customHeight="1">
       <c r="A24" t="s" s="7">
@@ -1724,10 +1840,18 @@
       <c r="B28" s="10">
         <v>520795</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="C28" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s" s="11">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" ht="20.35" customHeight="1">
       <c r="A29" t="s" s="7">
@@ -1784,10 +1908,18 @@
       <c r="B33" s="10">
         <v>485057</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
+      <c r="C33" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s" s="11">
+        <v>15</v>
+      </c>
     </row>
     <row r="34" ht="20.35" customHeight="1">
       <c r="A34" t="s" s="7">
@@ -1844,10 +1976,18 @@
       <c r="B38" s="10">
         <v>507795</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+      <c r="C38" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s" s="11">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s" s="11">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" ht="20.35" customHeight="1">
       <c r="A39" t="s" s="7">
@@ -1904,10 +2044,18 @@
       <c r="B43" s="10">
         <v>507061</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
+      <c r="C43" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s" s="11">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s" s="11">
+        <v>19</v>
+      </c>
     </row>
     <row r="44" ht="20.35" customHeight="1">
       <c r="A44" t="s" s="7">
@@ -1964,10 +2112,18 @@
       <c r="B48" s="10">
         <v>488442</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
+      <c r="C48" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s" s="11">
+        <v>15</v>
+      </c>
     </row>
     <row r="49" ht="20.35" customHeight="1">
       <c r="A49" t="s" s="7">
@@ -2024,10 +2180,18 @@
       <c r="B53" s="10">
         <v>510053</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
+      <c r="C53" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s" s="11">
+        <v>20</v>
+      </c>
     </row>
     <row r="54" ht="20.35" customHeight="1">
       <c r="A54" t="s" s="7">
@@ -2084,10 +2248,18 @@
       <c r="B58" s="10">
         <v>401222</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
+      <c r="C58" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F58" t="s" s="11">
+        <v>21</v>
+      </c>
     </row>
     <row r="59" ht="20.35" customHeight="1">
       <c r="A59" t="s" s="7">
@@ -2144,10 +2316,18 @@
       <c r="B63" s="10">
         <v>497168</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
+      <c r="C63" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s" s="11">
+        <v>16</v>
+      </c>
+      <c r="F63" t="s" s="11">
+        <v>22</v>
+      </c>
     </row>
     <row r="64" ht="20.35" customHeight="1">
       <c r="A64" t="s" s="7">
@@ -2204,10 +2384,18 @@
       <c r="B68" s="10">
         <v>500362</v>
       </c>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
+      <c r="C68" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s" s="11">
+        <v>23</v>
+      </c>
+      <c r="F68" t="s" s="11">
+        <v>24</v>
+      </c>
     </row>
     <row r="69" ht="20.35" customHeight="1">
       <c r="A69" t="s" s="7">
@@ -2264,14 +2452,22 @@
       <c r="B73" s="10">
         <v>406170</v>
       </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
+      <c r="C73" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="F73" t="s" s="11">
+        <v>25</v>
+      </c>
     </row>
     <row r="74" ht="20.35" customHeight="1">
       <c r="A74" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B74" s="8">
         <v>310667</v>
@@ -2283,7 +2479,7 @@
     </row>
     <row r="75" ht="20.35" customHeight="1">
       <c r="A75" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B75" s="8">
         <v>247524</v>
@@ -2295,7 +2491,7 @@
     </row>
     <row r="76" ht="20.35" customHeight="1">
       <c r="A76" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B76" s="8">
         <v>202464</v>
@@ -2307,7 +2503,7 @@
     </row>
     <row r="77" ht="20.35" customHeight="1">
       <c r="A77" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B77" s="8">
         <v>301305</v>
@@ -2319,19 +2515,27 @@
     </row>
     <row r="78" ht="20.35" customHeight="1">
       <c r="A78" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B78" s="10">
         <v>407115</v>
       </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
+      <c r="C78" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D78" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="F78" t="s" s="11">
+        <v>27</v>
+      </c>
     </row>
     <row r="79" ht="20.35" customHeight="1">
       <c r="A79" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B79" s="8">
         <v>270542</v>
@@ -2343,7 +2547,7 @@
     </row>
     <row r="80" ht="20.35" customHeight="1">
       <c r="A80" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B80" s="8">
         <v>242007</v>
@@ -2355,7 +2559,7 @@
     </row>
     <row r="81" ht="20.35" customHeight="1">
       <c r="A81" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B81" s="8">
         <v>229342</v>
@@ -2367,7 +2571,7 @@
     </row>
     <row r="82" ht="20.35" customHeight="1">
       <c r="A82" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B82" s="8">
         <v>271342</v>
@@ -2379,19 +2583,27 @@
     </row>
     <row r="83" ht="20.35" customHeight="1">
       <c r="A83" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B83" s="10">
         <v>521075</v>
       </c>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
+      <c r="C83" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D83" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E83" t="s" s="11">
+        <v>28</v>
+      </c>
+      <c r="F83" t="s" s="11">
+        <v>29</v>
+      </c>
     </row>
     <row r="84" ht="20.35" customHeight="1">
       <c r="A84" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B84" s="8">
         <v>212058</v>
@@ -2403,7 +2615,7 @@
     </row>
     <row r="85" ht="20.35" customHeight="1">
       <c r="A85" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B85" s="8">
         <v>228481</v>
@@ -2415,7 +2627,7 @@
     </row>
     <row r="86" ht="20.35" customHeight="1">
       <c r="A86" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B86" s="8">
         <v>279309</v>
@@ -2427,7 +2639,7 @@
     </row>
     <row r="87" ht="20.35" customHeight="1">
       <c r="A87" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B87" s="8">
         <v>204184</v>
@@ -2439,19 +2651,27 @@
     </row>
     <row r="88" ht="20.35" customHeight="1">
       <c r="A88" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B88" s="10">
         <v>309873</v>
       </c>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
+      <c r="C88" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D88" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E88" t="s" s="11">
+        <v>16</v>
+      </c>
+      <c r="F88" t="s" s="11">
+        <v>22</v>
+      </c>
     </row>
     <row r="89" ht="20.35" customHeight="1">
       <c r="A89" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B89" s="8">
         <v>299586</v>
@@ -2463,7 +2683,7 @@
     </row>
     <row r="90" ht="20.35" customHeight="1">
       <c r="A90" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B90" s="8">
         <v>301658</v>
@@ -2475,7 +2695,7 @@
     </row>
     <row r="91" ht="20.35" customHeight="1">
       <c r="A91" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B91" s="8">
         <v>233198</v>
@@ -2487,7 +2707,7 @@
     </row>
     <row r="92" ht="20.35" customHeight="1">
       <c r="A92" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B92" s="8">
         <v>407099</v>
@@ -2499,19 +2719,27 @@
     </row>
     <row r="93" ht="20.35" customHeight="1">
       <c r="A93" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B93" s="10">
         <v>311475</v>
       </c>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
-      <c r="F93" s="9"/>
+      <c r="C93" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D93" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="E93" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F93" t="s" s="11">
+        <v>15</v>
+      </c>
     </row>
     <row r="94" ht="20.35" customHeight="1">
       <c r="A94" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B94" s="8">
         <v>295399</v>
@@ -2523,7 +2751,7 @@
     </row>
     <row r="95" ht="20.35" customHeight="1">
       <c r="A95" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B95" s="8">
         <v>230314</v>
@@ -2535,7 +2763,7 @@
     </row>
     <row r="96" ht="20.35" customHeight="1">
       <c r="A96" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B96" s="8">
         <v>208965</v>
@@ -2547,7 +2775,7 @@
     </row>
     <row r="97" ht="20.35" customHeight="1">
       <c r="A97" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B97" s="8">
         <v>214937</v>
@@ -2559,19 +2787,27 @@
     </row>
     <row r="98" ht="20.35" customHeight="1">
       <c r="A98" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B98" s="10">
         <v>207493</v>
       </c>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-      <c r="E98" s="9"/>
-      <c r="F98" s="9"/>
+      <c r="C98" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="E98" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F98" t="s" s="11">
+        <v>15</v>
+      </c>
     </row>
     <row r="99" ht="20.35" customHeight="1">
       <c r="A99" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B99" s="8">
         <v>234036</v>
@@ -2583,7 +2819,7 @@
     </row>
     <row r="100" ht="20.35" customHeight="1">
       <c r="A100" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B100" s="8">
         <v>302283</v>
@@ -2595,7 +2831,7 @@
     </row>
     <row r="101" ht="20.35" customHeight="1">
       <c r="A101" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B101" s="8">
         <v>219214</v>
@@ -2607,7 +2843,7 @@
     </row>
     <row r="102" ht="20.35" customHeight="1">
       <c r="A102" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B102" s="8">
         <v>218623</v>
@@ -2619,19 +2855,27 @@
     </row>
     <row r="103" ht="20.35" customHeight="1">
       <c r="A103" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B103" s="10">
         <v>304843</v>
       </c>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9"/>
-      <c r="F103" s="9"/>
+      <c r="C103" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D103" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E103" t="s" s="11">
+        <v>28</v>
+      </c>
+      <c r="F103" t="s" s="11">
+        <v>30</v>
+      </c>
     </row>
     <row r="104" ht="20.35" customHeight="1">
       <c r="A104" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B104" s="8">
         <v>250184</v>
@@ -2643,7 +2887,7 @@
     </row>
     <row r="105" ht="20.35" customHeight="1">
       <c r="A105" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B105" s="8">
         <v>336246</v>
@@ -2655,7 +2899,7 @@
     </row>
     <row r="106" ht="20.35" customHeight="1">
       <c r="A106" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B106" s="8">
         <v>244628</v>
@@ -2667,7 +2911,7 @@
     </row>
     <row r="107" ht="20.35" customHeight="1">
       <c r="A107" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B107" s="8">
         <v>261637</v>
@@ -2679,19 +2923,27 @@
     </row>
     <row r="108" ht="20.35" customHeight="1">
       <c r="A108" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B108" s="10">
         <v>260625</v>
       </c>
-      <c r="C108" s="9"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="9"/>
+      <c r="C108" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D108" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E108" t="s" s="11">
+        <v>28</v>
+      </c>
+      <c r="F108" t="s" s="11">
+        <v>31</v>
+      </c>
     </row>
     <row r="109" ht="20.35" customHeight="1">
       <c r="A109" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B109" s="8">
         <v>221256</v>
@@ -2703,7 +2955,7 @@
     </row>
     <row r="110" ht="20.35" customHeight="1">
       <c r="A110" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B110" s="8">
         <v>210418</v>
@@ -2715,7 +2967,7 @@
     </row>
     <row r="111" ht="20.35" customHeight="1">
       <c r="A111" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B111" s="8">
         <v>233027</v>
@@ -2727,7 +2979,7 @@
     </row>
     <row r="112" ht="20.35" customHeight="1">
       <c r="A112" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B112" s="8">
         <v>235288</v>
@@ -2739,19 +2991,27 @@
     </row>
     <row r="113" ht="20.35" customHeight="1">
       <c r="A113" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B113" s="10">
         <v>214694</v>
       </c>
-      <c r="C113" s="9"/>
-      <c r="D113" s="9"/>
-      <c r="E113" s="9"/>
-      <c r="F113" s="9"/>
+      <c r="C113" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D113" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="E113" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F113" t="s" s="11">
+        <v>32</v>
+      </c>
     </row>
     <row r="114" ht="20.35" customHeight="1">
       <c r="A114" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B114" s="8">
         <v>284798</v>
@@ -2763,7 +3023,7 @@
     </row>
     <row r="115" ht="20.35" customHeight="1">
       <c r="A115" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B115" s="8">
         <v>212334</v>
@@ -2775,7 +3035,7 @@
     </row>
     <row r="116" ht="20.35" customHeight="1">
       <c r="A116" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B116" s="8">
         <v>313447</v>
@@ -2787,7 +3047,7 @@
     </row>
     <row r="117" ht="20.35" customHeight="1">
       <c r="A117" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B117" s="8">
         <v>207513</v>
@@ -2799,19 +3059,27 @@
     </row>
     <row r="118" ht="20.35" customHeight="1">
       <c r="A118" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B118" s="10">
         <v>228999</v>
       </c>
-      <c r="C118" s="9"/>
-      <c r="D118" s="9"/>
-      <c r="E118" s="9"/>
-      <c r="F118" s="9"/>
+      <c r="C118" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="D118" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E118" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F118" t="s" s="11">
+        <v>20</v>
+      </c>
     </row>
     <row r="119" ht="20.35" customHeight="1">
       <c r="A119" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B119" s="8">
         <v>211650</v>
@@ -2823,7 +3091,7 @@
     </row>
     <row r="120" ht="20.35" customHeight="1">
       <c r="A120" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B120" s="8">
         <v>256650</v>
@@ -2835,7 +3103,7 @@
     </row>
     <row r="121" ht="20.35" customHeight="1">
       <c r="A121" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B121" s="8">
         <v>272954</v>
@@ -2847,7 +3115,7 @@
     </row>
     <row r="122" ht="20.35" customHeight="1">
       <c r="A122" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B122" s="8">
         <v>300240</v>
@@ -2859,9 +3127,9 @@
     </row>
     <row r="123" ht="20.35" customHeight="1">
       <c r="A123" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B123" s="10">
+        <v>26</v>
+      </c>
+      <c r="B123" s="12">
         <v>250680</v>
       </c>
       <c r="C123" s="9"/>
@@ -2871,7 +3139,7 @@
     </row>
     <row r="124" ht="20.35" customHeight="1">
       <c r="A124" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B124" s="8">
         <v>219962</v>
@@ -2883,7 +3151,7 @@
     </row>
     <row r="125" ht="20.35" customHeight="1">
       <c r="A125" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B125" s="8">
         <v>232094</v>
@@ -2895,7 +3163,7 @@
     </row>
     <row r="126" ht="20.35" customHeight="1">
       <c r="A126" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B126" s="8">
         <v>218232</v>
@@ -2907,7 +3175,7 @@
     </row>
     <row r="127" ht="20.35" customHeight="1">
       <c r="A127" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B127" s="8">
         <v>291748</v>
@@ -2919,9 +3187,9 @@
     </row>
     <row r="128" ht="20.35" customHeight="1">
       <c r="A128" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B128" s="11">
+        <v>26</v>
+      </c>
+      <c r="B128" s="12">
         <v>252890</v>
       </c>
       <c r="C128" s="9"/>
@@ -2931,7 +3199,7 @@
     </row>
     <row r="129" ht="20.35" customHeight="1">
       <c r="A129" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B129" s="8">
         <v>224004</v>
@@ -2943,7 +3211,7 @@
     </row>
     <row r="130" ht="20.35" customHeight="1">
       <c r="A130" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B130" s="8">
         <v>250188</v>
@@ -2955,7 +3223,7 @@
     </row>
     <row r="131" ht="20.35" customHeight="1">
       <c r="A131" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B131" s="8">
         <v>274096</v>
@@ -2967,7 +3235,7 @@
     </row>
     <row r="132" ht="20.35" customHeight="1">
       <c r="A132" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B132" s="8">
         <v>242457</v>
@@ -2979,9 +3247,9 @@
     </row>
     <row r="133" ht="20.35" customHeight="1">
       <c r="A133" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B133" s="11">
+        <v>26</v>
+      </c>
+      <c r="B133" s="12">
         <v>310206</v>
       </c>
       <c r="C133" s="9"/>
@@ -2991,7 +3259,7 @@
     </row>
     <row r="134" ht="20.35" customHeight="1">
       <c r="A134" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B134" s="8">
         <v>234016</v>
@@ -3003,7 +3271,7 @@
     </row>
     <row r="135" ht="20.35" customHeight="1">
       <c r="A135" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B135" s="8">
         <v>210462</v>
@@ -3015,7 +3283,7 @@
     </row>
     <row r="136" ht="20.35" customHeight="1">
       <c r="A136" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B136" s="8">
         <v>218639</v>
@@ -3027,7 +3295,7 @@
     </row>
     <row r="137" ht="20.35" customHeight="1">
       <c r="A137" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B137" s="8">
         <v>331683</v>
@@ -3039,9 +3307,9 @@
     </row>
     <row r="138" ht="20.35" customHeight="1">
       <c r="A138" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B138" s="11">
+        <v>26</v>
+      </c>
+      <c r="B138" s="12">
         <v>218649</v>
       </c>
       <c r="C138" s="9"/>
@@ -3051,7 +3319,7 @@
     </row>
     <row r="139" ht="20.35" customHeight="1">
       <c r="A139" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B139" s="8">
         <v>258722</v>
@@ -3063,7 +3331,7 @@
     </row>
     <row r="140" ht="20.35" customHeight="1">
       <c r="A140" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B140" s="8">
         <v>203115</v>
@@ -3075,7 +3343,7 @@
     </row>
     <row r="141" ht="20.35" customHeight="1">
       <c r="A141" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B141" s="8">
         <v>249996</v>
@@ -3087,7 +3355,7 @@
     </row>
     <row r="142" ht="20.35" customHeight="1">
       <c r="A142" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B142" s="8">
         <v>269978</v>
@@ -3099,9 +3367,9 @@
     </row>
     <row r="143" ht="20.35" customHeight="1">
       <c r="A143" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B143" s="11">
+        <v>26</v>
+      </c>
+      <c r="B143" s="12">
         <v>275089</v>
       </c>
       <c r="C143" s="9"/>
@@ -3111,7 +3379,7 @@
     </row>
     <row r="144" ht="20.35" customHeight="1">
       <c r="A144" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B144" s="8">
         <v>215930</v>
@@ -3123,7 +3391,7 @@
     </row>
     <row r="145" ht="20.35" customHeight="1">
       <c r="A145" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B145" s="8">
         <v>264724</v>
@@ -3135,7 +3403,7 @@
     </row>
     <row r="146" ht="20.35" customHeight="1">
       <c r="A146" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B146" s="8">
         <v>525734</v>
@@ -3147,7 +3415,7 @@
     </row>
     <row r="147" ht="20.35" customHeight="1">
       <c r="A147" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B147" s="8">
         <v>421798</v>
@@ -3159,9 +3427,9 @@
     </row>
     <row r="148" ht="20.35" customHeight="1">
       <c r="A148" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B148" s="11">
+        <v>26</v>
+      </c>
+      <c r="B148" s="12">
         <v>306439</v>
       </c>
       <c r="C148" s="9"/>
@@ -3171,7 +3439,7 @@
     </row>
     <row r="149" ht="20.35" customHeight="1">
       <c r="A149" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B149" s="8">
         <v>255724</v>
@@ -3183,7 +3451,7 @@
     </row>
     <row r="150" ht="20.35" customHeight="1">
       <c r="A150" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B150" s="8">
         <v>235526</v>
@@ -3195,7 +3463,7 @@
     </row>
     <row r="151" ht="20.35" customHeight="1">
       <c r="A151" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B151" s="8">
         <v>304895</v>
@@ -3207,7 +3475,7 @@
     </row>
     <row r="152" ht="20.35" customHeight="1">
       <c r="A152" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B152" s="8">
         <v>254931</v>
@@ -3219,9 +3487,9 @@
     </row>
     <row r="153" ht="20.35" customHeight="1">
       <c r="A153" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B153" s="11">
+        <v>26</v>
+      </c>
+      <c r="B153" s="12">
         <v>229305</v>
       </c>
       <c r="C153" s="9"/>
@@ -3231,7 +3499,7 @@
     </row>
     <row r="154" ht="20.35" customHeight="1">
       <c r="A154" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B154" s="8">
         <v>212662</v>
@@ -3243,7 +3511,7 @@
     </row>
     <row r="155" ht="20.35" customHeight="1">
       <c r="A155" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B155" s="8">
         <v>525516</v>
@@ -3255,7 +3523,7 @@
     </row>
     <row r="156" ht="20.35" customHeight="1">
       <c r="A156" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B156" s="8">
         <v>210685</v>
@@ -3267,7 +3535,7 @@
     </row>
     <row r="157" ht="20.35" customHeight="1">
       <c r="A157" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B157" s="8">
         <v>215406</v>
@@ -3279,9 +3547,9 @@
     </row>
     <row r="158" ht="20.35" customHeight="1">
       <c r="A158" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B158" s="11">
+        <v>26</v>
+      </c>
+      <c r="B158" s="12">
         <v>210670</v>
       </c>
       <c r="C158" s="9"/>
@@ -3291,7 +3559,7 @@
     </row>
     <row r="159" ht="20.35" customHeight="1">
       <c r="A159" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B159" s="8">
         <v>253224</v>
@@ -3303,7 +3571,7 @@
     </row>
     <row r="160" ht="20.35" customHeight="1">
       <c r="A160" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B160" s="8">
         <v>305334</v>
@@ -3315,7 +3583,7 @@
     </row>
     <row r="161" ht="20.35" customHeight="1">
       <c r="A161" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B161" s="8">
         <v>212336</v>
@@ -3327,7 +3595,7 @@
     </row>
     <row r="162" ht="20.35" customHeight="1">
       <c r="A162" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B162" s="8">
         <v>233761</v>
@@ -3339,9 +3607,9 @@
     </row>
     <row r="163" ht="20.35" customHeight="1">
       <c r="A163" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B163" s="11">
+        <v>26</v>
+      </c>
+      <c r="B163" s="12">
         <v>303990</v>
       </c>
       <c r="C163" s="9"/>
@@ -3351,7 +3619,7 @@
     </row>
     <row r="164" ht="20.35" customHeight="1">
       <c r="A164" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B164" s="8">
         <v>266939</v>
@@ -3363,7 +3631,7 @@
     </row>
     <row r="165" ht="20.35" customHeight="1">
       <c r="A165" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B165" s="8">
         <v>219224</v>
@@ -3375,7 +3643,7 @@
     </row>
     <row r="166" ht="20.35" customHeight="1">
       <c r="A166" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B166" s="8">
         <v>343329</v>
@@ -3387,7 +3655,7 @@
     </row>
     <row r="167" ht="20.35" customHeight="1">
       <c r="A167" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B167" s="8">
         <v>211934</v>
@@ -3399,9 +3667,9 @@
     </row>
     <row r="168" ht="20.35" customHeight="1">
       <c r="A168" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B168" s="11">
+        <v>26</v>
+      </c>
+      <c r="B168" s="12">
         <v>221513</v>
       </c>
       <c r="C168" s="9"/>
@@ -3411,7 +3679,7 @@
     </row>
     <row r="169" ht="20.35" customHeight="1">
       <c r="A169" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B169" s="8">
         <v>299818</v>
@@ -3423,7 +3691,7 @@
     </row>
     <row r="170" ht="20.35" customHeight="1">
       <c r="A170" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B170" s="8">
         <v>406986</v>
@@ -3435,7 +3703,7 @@
     </row>
     <row r="171" ht="20.35" customHeight="1">
       <c r="A171" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B171" s="8">
         <v>229066</v>
@@ -3447,7 +3715,7 @@
     </row>
     <row r="172" ht="20.35" customHeight="1">
       <c r="A172" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B172" s="8">
         <v>320613</v>
@@ -3459,9 +3727,9 @@
     </row>
     <row r="173" ht="20.35" customHeight="1">
       <c r="A173" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B173" s="11">
+        <v>26</v>
+      </c>
+      <c r="B173" s="12">
         <v>218532</v>
       </c>
       <c r="C173" s="9"/>
@@ -3471,7 +3739,7 @@
     </row>
     <row r="174" ht="20.35" customHeight="1">
       <c r="A174" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B174" s="8">
         <v>225018</v>
@@ -3483,7 +3751,7 @@
     </row>
     <row r="175" ht="20.35" customHeight="1">
       <c r="A175" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B175" s="8">
         <v>257431</v>
@@ -3495,7 +3763,7 @@
     </row>
     <row r="176" ht="20.35" customHeight="1">
       <c r="A176" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B176" s="8">
         <v>369834</v>
@@ -3507,7 +3775,7 @@
     </row>
     <row r="177" ht="20.35" customHeight="1">
       <c r="A177" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B177" s="8">
         <v>300928</v>
@@ -3519,9 +3787,9 @@
     </row>
     <row r="178" ht="20.35" customHeight="1">
       <c r="A178" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B178" s="11">
+        <v>26</v>
+      </c>
+      <c r="B178" s="12">
         <v>325611</v>
       </c>
       <c r="C178" s="9"/>
@@ -3531,7 +3799,7 @@
     </row>
     <row r="179" ht="20.35" customHeight="1">
       <c r="A179" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B179" s="8">
         <v>216433</v>
@@ -3543,7 +3811,7 @@
     </row>
     <row r="180" ht="20.35" customHeight="1">
       <c r="A180" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B180" s="8">
         <v>345209</v>
@@ -3555,7 +3823,7 @@
     </row>
     <row r="181" ht="20.35" customHeight="1">
       <c r="A181" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B181" s="8">
         <v>275975</v>
@@ -3567,7 +3835,7 @@
     </row>
     <row r="182" ht="20.35" customHeight="1">
       <c r="A182" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B182" s="8">
         <v>202985</v>
@@ -3579,9 +3847,9 @@
     </row>
     <row r="183" ht="20.35" customHeight="1">
       <c r="A183" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B183" s="11">
+        <v>26</v>
+      </c>
+      <c r="B183" s="12">
         <v>179317</v>
       </c>
       <c r="C183" s="9"/>
@@ -3591,7 +3859,7 @@
     </row>
     <row r="184" ht="20.35" customHeight="1">
       <c r="A184" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B184" s="8">
         <v>229877</v>
@@ -3603,7 +3871,7 @@
     </row>
     <row r="185" ht="20.35" customHeight="1">
       <c r="A185" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B185" s="8">
         <v>209852</v>
@@ -3615,7 +3883,7 @@
     </row>
     <row r="186" ht="20.35" customHeight="1">
       <c r="A186" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B186" s="8">
         <v>514863</v>
@@ -3627,7 +3895,7 @@
     </row>
     <row r="187" ht="20.35" customHeight="1">
       <c r="A187" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B187" s="8">
         <v>209549</v>
@@ -3639,9 +3907,9 @@
     </row>
     <row r="188" ht="20.35" customHeight="1">
       <c r="A188" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B188" s="11">
+        <v>26</v>
+      </c>
+      <c r="B188" s="12">
         <v>272483</v>
       </c>
       <c r="C188" s="9"/>
@@ -3651,7 +3919,7 @@
     </row>
     <row r="189" ht="20.35" customHeight="1">
       <c r="A189" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B189" s="8">
         <v>400854</v>
@@ -3663,7 +3931,7 @@
     </row>
     <row r="190" ht="20.35" customHeight="1">
       <c r="A190" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B190" s="8">
         <v>302278</v>
@@ -3675,7 +3943,7 @@
     </row>
     <row r="191" ht="20.35" customHeight="1">
       <c r="A191" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B191" s="8">
         <v>525796</v>
@@ -3687,7 +3955,7 @@
     </row>
     <row r="192" ht="20.35" customHeight="1">
       <c r="A192" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B192" s="8">
         <v>263546</v>
@@ -3699,9 +3967,9 @@
     </row>
     <row r="193" ht="20.35" customHeight="1">
       <c r="A193" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B193" s="11">
+        <v>26</v>
+      </c>
+      <c r="B193" s="12">
         <v>262611</v>
       </c>
       <c r="C193" s="9"/>
@@ -3711,7 +3979,7 @@
     </row>
     <row r="194" ht="20.35" customHeight="1">
       <c r="A194" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B194" s="8">
         <v>232413</v>
@@ -3723,7 +3991,7 @@
     </row>
     <row r="195" ht="20.35" customHeight="1">
       <c r="A195" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B195" s="8">
         <v>436872</v>
@@ -3735,7 +4003,7 @@
     </row>
     <row r="196" ht="20.35" customHeight="1">
       <c r="A196" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B196" s="8">
         <v>247377</v>
@@ -3747,7 +4015,7 @@
     </row>
     <row r="197" ht="20.35" customHeight="1">
       <c r="A197" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B197" s="8">
         <v>220786</v>
@@ -3759,9 +4027,9 @@
     </row>
     <row r="198" ht="20.35" customHeight="1">
       <c r="A198" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B198" s="11">
+        <v>26</v>
+      </c>
+      <c r="B198" s="12">
         <v>204290</v>
       </c>
       <c r="C198" s="9"/>
@@ -3771,7 +4039,7 @@
     </row>
     <row r="199" ht="20.35" customHeight="1">
       <c r="A199" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B199" s="8">
         <v>258132</v>
@@ -3783,7 +4051,7 @@
     </row>
     <row r="200" ht="20.35" customHeight="1">
       <c r="A200" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B200" s="8">
         <v>304942</v>
@@ -3795,7 +4063,7 @@
     </row>
     <row r="201" ht="20.35" customHeight="1">
       <c r="A201" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B201" s="8">
         <v>222501</v>
@@ -3807,7 +4075,7 @@
     </row>
     <row r="202" ht="20.35" customHeight="1">
       <c r="A202" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B202" s="8">
         <v>207976</v>
@@ -3819,9 +4087,9 @@
     </row>
     <row r="203" ht="20.35" customHeight="1">
       <c r="A203" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B203" s="11">
+        <v>26</v>
+      </c>
+      <c r="B203" s="12">
         <v>263487</v>
       </c>
       <c r="C203" s="9"/>
@@ -3831,7 +4099,7 @@
     </row>
     <row r="204" ht="20.35" customHeight="1">
       <c r="A204" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B204" s="8">
         <v>495726</v>
@@ -3843,7 +4111,7 @@
     </row>
     <row r="205" ht="20.35" customHeight="1">
       <c r="A205" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B205" s="8">
         <v>181297</v>
@@ -3855,7 +4123,7 @@
     </row>
     <row r="206" ht="20.35" customHeight="1">
       <c r="A206" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B206" s="8">
         <v>225250</v>
@@ -3867,7 +4135,7 @@
     </row>
     <row r="207" ht="20.35" customHeight="1">
       <c r="A207" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B207" s="8">
         <v>306279</v>
@@ -3879,9 +4147,9 @@
     </row>
     <row r="208" ht="20.35" customHeight="1">
       <c r="A208" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B208" s="11">
+        <v>26</v>
+      </c>
+      <c r="B208" s="12">
         <v>272795</v>
       </c>
       <c r="C208" s="9"/>
@@ -3891,7 +4159,7 @@
     </row>
     <row r="209" ht="20.35" customHeight="1">
       <c r="A209" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B209" s="8">
         <v>516095</v>
@@ -3903,7 +4171,7 @@
     </row>
     <row r="210" ht="20.35" customHeight="1">
       <c r="A210" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B210" s="8">
         <v>212607</v>
@@ -3915,7 +4183,7 @@
     </row>
     <row r="211" ht="20.35" customHeight="1">
       <c r="A211" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B211" s="8">
         <v>274319</v>
@@ -3927,7 +4195,7 @@
     </row>
     <row r="212" ht="20.35" customHeight="1">
       <c r="A212" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B212" s="8">
         <v>222639</v>
@@ -3939,9 +4207,9 @@
     </row>
     <row r="213" ht="20.35" customHeight="1">
       <c r="A213" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B213" s="11">
+        <v>26</v>
+      </c>
+      <c r="B213" s="12">
         <v>325095</v>
       </c>
       <c r="C213" s="9"/>
@@ -3951,7 +4219,7 @@
     </row>
     <row r="214" ht="20.35" customHeight="1">
       <c r="A214" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B214" s="8">
         <v>217927</v>
@@ -3963,7 +4231,7 @@
     </row>
     <row r="215" ht="20.35" customHeight="1">
       <c r="A215" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B215" s="8">
         <v>334519</v>
@@ -3975,7 +4243,7 @@
     </row>
     <row r="216" ht="20.35" customHeight="1">
       <c r="A216" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B216" s="8">
         <v>226116</v>
@@ -3987,7 +4255,7 @@
     </row>
     <row r="217" ht="20.35" customHeight="1">
       <c r="A217" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B217" s="8">
         <v>217100</v>
@@ -3999,9 +4267,9 @@
     </row>
     <row r="218" ht="20.35" customHeight="1">
       <c r="A218" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B218" s="11">
+        <v>26</v>
+      </c>
+      <c r="B218" s="12">
         <v>247058</v>
       </c>
       <c r="C218" s="9"/>
@@ -4011,7 +4279,7 @@
     </row>
     <row r="219" ht="20.35" customHeight="1">
       <c r="A219" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B219" s="8">
         <v>289866</v>
@@ -4023,7 +4291,7 @@
     </row>
     <row r="220" ht="20.35" customHeight="1">
       <c r="A220" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B220" s="8">
         <v>279015</v>
@@ -4035,7 +4303,7 @@
     </row>
     <row r="221" ht="20.35" customHeight="1">
       <c r="A221" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B221" s="8">
         <v>209680</v>
@@ -4047,7 +4315,7 @@
     </row>
     <row r="222" ht="20.35" customHeight="1">
       <c r="A222" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B222" s="8">
         <v>358842</v>
@@ -4059,9 +4327,9 @@
     </row>
     <row r="223" ht="20.35" customHeight="1">
       <c r="A223" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B223" s="11">
+        <v>26</v>
+      </c>
+      <c r="B223" s="12">
         <v>222957</v>
       </c>
       <c r="C223" s="9"/>
@@ -4071,7 +4339,7 @@
     </row>
     <row r="224" ht="20.35" customHeight="1">
       <c r="A224" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B224" s="8">
         <v>218741</v>
@@ -4083,7 +4351,7 @@
     </row>
     <row r="225" ht="20.35" customHeight="1">
       <c r="A225" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B225" s="8">
         <v>205447</v>
@@ -4095,7 +4363,7 @@
     </row>
     <row r="226" ht="20.35" customHeight="1">
       <c r="A226" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B226" s="8">
         <v>232632</v>
@@ -4107,7 +4375,7 @@
     </row>
     <row r="227" ht="20.35" customHeight="1">
       <c r="A227" t="s" s="7">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B227" s="8">
         <v>422026</v>
@@ -4119,9 +4387,9 @@
     </row>
     <row r="228" ht="20.35" customHeight="1">
       <c r="A228" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="B228" s="11">
+        <v>26</v>
+      </c>
+      <c r="B228" s="12">
         <v>220280</v>
       </c>
       <c r="C228" s="9"/>
@@ -4131,7 +4399,7 @@
     </row>
     <row r="229" ht="20.35" customHeight="1">
       <c r="A229" t="s" s="7">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B229" s="8">
         <v>518542</v>
@@ -4143,7 +4411,7 @@
     </row>
     <row r="230" ht="20.35" customHeight="1">
       <c r="A230" t="s" s="7">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B230" s="8">
         <v>314622</v>
@@ -4155,7 +4423,7 @@
     </row>
     <row r="231" ht="20.35" customHeight="1">
       <c r="A231" t="s" s="7">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B231" s="8">
         <v>444725</v>
@@ -4167,7 +4435,7 @@
     </row>
     <row r="232" ht="20.35" customHeight="1">
       <c r="A232" t="s" s="7">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B232" s="8">
         <v>441791</v>
@@ -4179,9 +4447,9 @@
     </row>
     <row r="233" ht="20.35" customHeight="1">
       <c r="A233" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="B233" s="11">
+        <v>33</v>
+      </c>
+      <c r="B233" s="12">
         <v>487493</v>
       </c>
       <c r="C233" s="9"/>
@@ -4191,7 +4459,7 @@
     </row>
     <row r="234" ht="20.35" customHeight="1">
       <c r="A234" t="s" s="7">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B234" s="8">
         <v>476529</v>
@@ -4203,7 +4471,7 @@
     </row>
     <row r="235" ht="20.35" customHeight="1">
       <c r="A235" t="s" s="7">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B235" s="8">
         <v>490853</v>

</xml_diff>